<commit_message>
ran experiments with diff prompts
</commit_message>
<xml_diff>
--- a/benchmarking_outputs/onlyPhaseOne20251119_162053.xlsx
+++ b/benchmarking_outputs/onlyPhaseOne20251119_162053.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rastegar-a/Documents/GitHub/i-adopt-llm-based-service/benchmarking_outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4AEB39-A9F9-7643-93D6-62C5C5FFDA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30D11FB-07C6-2D42-BF79-C40225E7980D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2957,14 +2957,21 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2994,7 +3001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3003,6 +3010,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8593,7 +8603,7 @@
   <dimension ref="A1:AT4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AQ2" sqref="AQ2"/>
+      <selection activeCell="G4" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8757,7 +8767,7 @@
       <c r="F2" s="3">
         <v>0.85</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>0.55900000000000005</v>
       </c>
       <c r="H2" s="3">
@@ -8897,7 +8907,7 @@
       <c r="F3" s="3">
         <v>0.82599999999999996</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="4">
         <v>0.52</v>
       </c>
       <c r="H3" s="3">
@@ -9037,7 +9047,7 @@
       <c r="F4" s="3">
         <v>0.83299999999999996</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="4">
         <v>0.496</v>
       </c>
       <c r="H4" s="3">

</xml_diff>